<commit_message>
Almost done, I write report
</commit_message>
<xml_diff>
--- a/statistics/random_walk/gathered.xlsx
+++ b/statistics/random_walk/gathered.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\ForumPolarization\statistics\random_walk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E78A77C-C27A-4AEA-BBD6-94B156A539A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00940E1A-8623-48BC-8CE0-F5A1B1E8305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -637,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -743,10 +743,16 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="28" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -757,13 +763,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -4379,8 +4378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:X82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80:E82"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L71" sqref="L71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,45 +4397,45 @@
       </c>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B3" s="90" t="s">
+      <c r="B3" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="91" t="s">
+      <c r="C3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91" t="s">
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="91"/>
-      <c r="H3" s="91"/>
-      <c r="I3" s="91" t="s">
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="91"/>
-      <c r="K3" s="91"/>
-      <c r="N3" s="90" t="s">
+      <c r="J3" s="90"/>
+      <c r="K3" s="90"/>
+      <c r="N3" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="91" t="s">
+      <c r="O3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="91"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="91" t="s">
+      <c r="P3" s="90"/>
+      <c r="Q3" s="90"/>
+      <c r="R3" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="91"/>
-      <c r="T3" s="91"/>
-      <c r="U3" s="91" t="s">
+      <c r="S3" s="90"/>
+      <c r="T3" s="90"/>
+      <c r="U3" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="91"/>
-      <c r="W3" s="91"/>
+      <c r="V3" s="90"/>
+      <c r="W3" s="90"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="90"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
@@ -4464,7 +4463,7 @@
       <c r="K4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="90"/>
+      <c r="N4" s="93"/>
       <c r="O4" s="1" t="s">
         <v>4</v>
       </c>
@@ -5052,45 +5051,45 @@
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B22" s="90" t="s">
+      <c r="B22" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="91" t="s">
+      <c r="C22" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D22" s="91"/>
-      <c r="E22" s="91"/>
-      <c r="F22" s="91" t="s">
+      <c r="D22" s="90"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="91"/>
-      <c r="H22" s="91"/>
-      <c r="I22" s="91" t="s">
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="J22" s="91"/>
-      <c r="K22" s="91"/>
-      <c r="N22" s="95" t="s">
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="N22" s="91" t="s">
         <v>0</v>
       </c>
-      <c r="O22" s="92" t="s">
+      <c r="O22" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="P22" s="93"/>
-      <c r="Q22" s="94"/>
-      <c r="R22" s="92" t="s">
+      <c r="P22" s="95"/>
+      <c r="Q22" s="96"/>
+      <c r="R22" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="S22" s="93"/>
-      <c r="T22" s="94"/>
-      <c r="U22" s="92" t="s">
+      <c r="S22" s="95"/>
+      <c r="T22" s="96"/>
+      <c r="U22" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="V22" s="93"/>
-      <c r="W22" s="94"/>
+      <c r="V22" s="95"/>
+      <c r="W22" s="96"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B23" s="90"/>
+      <c r="B23" s="93"/>
       <c r="C23" s="1" t="s">
         <v>4</v>
       </c>
@@ -5118,7 +5117,7 @@
       <c r="K23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N23" s="96"/>
+      <c r="N23" s="92"/>
       <c r="O23" s="5" t="s">
         <v>4</v>
       </c>
@@ -5706,45 +5705,45 @@
       </c>
     </row>
     <row r="41" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B41" s="90" t="s">
+      <c r="B41" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="91" t="s">
+      <c r="C41" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="91"/>
-      <c r="E41" s="91"/>
-      <c r="F41" s="91" t="s">
+      <c r="D41" s="90"/>
+      <c r="E41" s="90"/>
+      <c r="F41" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="91" t="s">
+      <c r="G41" s="90"/>
+      <c r="H41" s="90"/>
+      <c r="I41" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="J41" s="91"/>
-      <c r="K41" s="91"/>
-      <c r="N41" s="90" t="s">
+      <c r="J41" s="90"/>
+      <c r="K41" s="90"/>
+      <c r="N41" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="O41" s="91" t="s">
+      <c r="O41" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="P41" s="91"/>
-      <c r="Q41" s="91"/>
-      <c r="R41" s="91" t="s">
+      <c r="P41" s="90"/>
+      <c r="Q41" s="90"/>
+      <c r="R41" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="S41" s="91"/>
-      <c r="T41" s="91"/>
-      <c r="U41" s="91" t="s">
+      <c r="S41" s="90"/>
+      <c r="T41" s="90"/>
+      <c r="U41" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="V41" s="91"/>
-      <c r="W41" s="91"/>
+      <c r="V41" s="90"/>
+      <c r="W41" s="90"/>
     </row>
     <row r="42" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B42" s="90"/>
+      <c r="B42" s="93"/>
       <c r="C42" s="1" t="s">
         <v>4</v>
       </c>
@@ -5772,7 +5771,7 @@
       <c r="K42" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N42" s="90"/>
+      <c r="N42" s="93"/>
       <c r="O42" s="1" t="s">
         <v>4</v>
       </c>
@@ -6393,11 +6392,11 @@
       <c r="B81" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C81" s="97">
+      <c r="C81">
         <f>AVERAGE(C5:E13,C24:E32,C43:E51)</f>
         <v>0.52079629629629642</v>
       </c>
-      <c r="D81" s="97">
+      <c r="D81">
         <f>AVERAGE(F5:H13,F24:H32,F43:H51)</f>
         <v>0.58931604938271576</v>
       </c>
@@ -6425,6 +6424,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="R3:T3"/>
+    <mergeCell ref="U3:W3"/>
+    <mergeCell ref="O22:Q22"/>
+    <mergeCell ref="R22:T22"/>
+    <mergeCell ref="U22:W22"/>
     <mergeCell ref="O41:Q41"/>
     <mergeCell ref="R41:T41"/>
     <mergeCell ref="U41:W41"/>
@@ -6438,17 +6448,6 @@
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="R3:T3"/>
-    <mergeCell ref="U3:W3"/>
-    <mergeCell ref="O22:Q22"/>
-    <mergeCell ref="R22:T22"/>
-    <mergeCell ref="U22:W22"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:K3"/>
-    <mergeCell ref="N3:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>